<commit_message>
it won't be the end, never
</commit_message>
<xml_diff>
--- a/_figure/orders-of-growth.xlsx
+++ b/_figure/orders-of-growth.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -20,11 +20,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -32,7 +32,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -40,14 +40,20 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -89,13 +95,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -105,7 +111,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -142,6 +148,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -150,6 +166,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -191,7 +217,7 @@
                 <a:pPr>
                   <a:defRPr sz="1600"/>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -301,6 +327,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -309,6 +345,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -351,7 +397,7 @@
                 <a:pPr>
                   <a:defRPr sz="1600"/>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -461,6 +507,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -469,6 +525,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -510,7 +576,7 @@
                 <a:pPr>
                   <a:defRPr sz="1600"/>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -620,6 +686,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -628,6 +704,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -665,7 +751,7 @@
                 <a:pPr>
                   <a:defRPr sz="1600"/>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -775,6 +861,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -796,7 +892,7 @@
                 <a:pPr>
                   <a:defRPr sz="1600"/>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -906,6 +1002,16 @@
             <c:marker>
               <c:symbol val="circle"/>
               <c:size val="7"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                  <a:noFill/>
+                  <a:prstDash val="solid"/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
           </c:dPt>
@@ -927,7 +1033,7 @@
                 <a:pPr>
                   <a:defRPr sz="1600"/>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="zh-CN"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1120,11 +1226,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2139598760"/>
-        <c:axId val="2139604632"/>
+        <c:axId val="-2079541864"/>
+        <c:axId val="-2079901112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2139598760"/>
+        <c:axId val="-2079541864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10.0"/>
@@ -1171,6 +1277,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1178,15 +1291,15 @@
             <a:pPr>
               <a:defRPr sz="1600"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139604632"/>
+        <c:crossAx val="-2079901112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2139604632"/>
+        <c:axId val="-2079901112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="35.0"/>
@@ -1198,6 +1311,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -1205,10 +1325,10 @@
             <a:pPr>
               <a:defRPr sz="1600"/>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139598760"/>
+        <c:crossAx val="-2079541864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2668,7 +2788,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2993,10 +3113,11 @@
         <v>3628800</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="20">
+    <row r="16" spans="1:14" ht="19">
       <c r="N16" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>